<commit_message>
User Story 21 and accompanying tests
</commit_message>
<xml_diff>
--- a/khrwhjvtReport-2.xlsx
+++ b/khrwhjvtReport-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rweis\OneDrive\Stevens\SSW 555 - Agile\ssw555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="5E468C1BB0B3FB08B77CB2336C5D4C315534BE14" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{1D9CDDB5-E3A9-431A-8258-96D399C7BC7A}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="5E468C1BB0B3FB08B77CB2336C5D4C315534BE14" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{2E80B885-34C2-423D-8B68-8528293FA483}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="463" windowWidth="23040" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="463" windowWidth="23040" windowHeight="13183" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -867,7 +867,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -916,6 +916,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3311,7 +3312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -3621,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -3679,6 +3680,15 @@
       </c>
       <c r="F2" s="23">
         <v>30</v>
+      </c>
+      <c r="G2" s="23">
+        <v>20</v>
+      </c>
+      <c r="H2" s="24">
+        <v>60</v>
+      </c>
+      <c r="I2" s="30">
+        <v>41571</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3923,8 +3933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added User Story 22 with accompanying unit tests and updated Excel Spreadsheet
</commit_message>
<xml_diff>
--- a/khrwhjvtReport-2.xlsx
+++ b/khrwhjvtReport-2.xlsx
@@ -5,19 +5,19 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rweis\OneDrive\Stevens\SSW 555 - Agile\ssw555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d58f14bcaf2f6a6/Stevens/SSW 555 - Agile/ssw555/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="5E468C1BB0B3FB08B77CB2336C5D4C315534BE14" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{2E80B885-34C2-423D-8B68-8528293FA483}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="5E468C1BB0B3FB08B77CB2336C5D4C315534BE14" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{1C3EF1E3-67D2-4118-A94C-B5998DABCA5E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="463" windowWidth="23040" windowHeight="13183" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="463" windowWidth="15634" windowHeight="6874" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="Burndown README" sheetId="13" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="3" r:id="rId4"/>
-    <sheet name="Burndown" sheetId="7" r:id="rId5"/>
+    <sheet name="Burndown" sheetId="7" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="3" r:id="rId5"/>
     <sheet name="Sprint2" sheetId="4" r:id="rId6"/>
     <sheet name="Sprint3" sheetId="5" r:id="rId7"/>
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="218">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -708,6 +708,18 @@
   </si>
   <si>
     <t>Integrating in order</t>
+  </si>
+  <si>
+    <t>Completing work before deadlines</t>
+  </si>
+  <si>
+    <t>Communicating changes that have dependencies</t>
+  </si>
+  <si>
+    <t>Communicating status of work</t>
+  </si>
+  <si>
+    <t>Writing bad unit tests</t>
   </si>
 </sst>
 </file>
@@ -867,7 +879,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -917,6 +929,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2188,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -2230,6 +2245,9 @@
       <c r="C2" t="s">
         <v>157</v>
       </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
       <c r="E2" t="s">
         <v>199</v>
       </c>
@@ -2286,6 +2304,9 @@
       <c r="C6" t="s">
         <v>71</v>
       </c>
+      <c r="D6" t="s">
+        <v>183</v>
+      </c>
       <c r="E6" t="s">
         <v>199</v>
       </c>
@@ -2300,6 +2321,9 @@
       <c r="C7" t="s">
         <v>72</v>
       </c>
+      <c r="D7" t="s">
+        <v>183</v>
+      </c>
       <c r="E7" t="s">
         <v>199</v>
       </c>
@@ -2334,7 +2358,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>122</v>
@@ -2361,9 +2385,6 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
-      </c>
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -2375,9 +2396,6 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -2426,14 +2444,14 @@
       <c r="C16" t="s">
         <v>82</v>
       </c>
+      <c r="D16" t="s">
+        <v>183</v>
+      </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>3</v>
-      </c>
       <c r="B17" t="s">
         <v>129</v>
       </c>
@@ -2445,9 +2463,6 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>3</v>
-      </c>
       <c r="B18" t="s">
         <v>130</v>
       </c>
@@ -2459,9 +2474,6 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>3</v>
-      </c>
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -2473,9 +2485,6 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>3</v>
-      </c>
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -2487,9 +2496,6 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>3</v>
-      </c>
       <c r="B21" t="s">
         <v>133</v>
       </c>
@@ -2510,8 +2516,11 @@
       <c r="C22" t="s">
         <v>88</v>
       </c>
+      <c r="D22" t="s">
+        <v>183</v>
+      </c>
       <c r="E22" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2524,8 +2533,11 @@
       <c r="C23" t="s">
         <v>91</v>
       </c>
+      <c r="D23" t="s">
+        <v>183</v>
+      </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2543,9 +2555,6 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>4</v>
-      </c>
       <c r="B25" t="s">
         <v>137</v>
       </c>
@@ -2558,7 +2567,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
         <v>138</v>
@@ -2571,9 +2580,6 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>4</v>
-      </c>
       <c r="B27" t="s">
         <v>139</v>
       </c>
@@ -2586,7 +2592,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>140</v>
@@ -2600,7 +2606,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>141</v>
@@ -2614,7 +2620,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>142</v>
@@ -2627,9 +2633,6 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>4</v>
-      </c>
       <c r="B31" t="s">
         <v>143</v>
       </c>
@@ -2642,7 +2645,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>144</v>
@@ -2655,9 +2658,6 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>4</v>
-      </c>
       <c r="B33" t="s">
         <v>145</v>
       </c>
@@ -2665,6 +2665,34 @@
         <v>101</v>
       </c>
       <c r="E33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2846,6 +2874,93 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" customWidth="1"/>
+    <col min="4" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>41542</v>
+      </c>
+      <c r="B2" s="17">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="16">
+        <v>170</v>
+      </c>
+      <c r="E2" s="16">
+        <v>545</v>
+      </c>
+      <c r="F2" s="9">
+        <f>D2/(E2/60)</f>
+        <v>18.715596330275229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>41548</v>
+      </c>
+      <c r="B3" s="18">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="16">
+        <v>102</v>
+      </c>
+      <c r="E3" s="16">
+        <v>325</v>
+      </c>
+      <c r="F3" s="9">
+        <f>D3/(E3/60)</f>
+        <v>18.830769230769231</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -3221,99 +3336,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="18.1328125" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
-        <v>41542</v>
-      </c>
-      <c r="B2" s="17">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2" s="16">
-        <v>170</v>
-      </c>
-      <c r="E2" s="16">
-        <v>545</v>
-      </c>
-      <c r="F2" s="9">
-        <f>D2/(E2/60)</f>
-        <v>18.715596330275229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <v>41548</v>
-      </c>
-      <c r="B3" s="18">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" s="16">
-        <v>102</v>
-      </c>
-      <c r="E3" s="16">
-        <v>325</v>
-      </c>
-      <c r="F3" s="9">
-        <f>D3/(E3/60)</f>
-        <v>18.830769230769231</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B25" sqref="B14:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -3620,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -3672,8 +3700,8 @@
       <c r="C2" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>156</v>
+      <c r="D2" s="24" t="s">
+        <v>199</v>
       </c>
       <c r="E2" s="23">
         <v>10</v>
@@ -3701,14 +3729,23 @@
       <c r="C3" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>156</v>
+      <c r="D3" s="24" t="s">
+        <v>199</v>
       </c>
       <c r="E3" s="23">
         <v>15</v>
       </c>
       <c r="F3" s="23">
         <v>40</v>
+      </c>
+      <c r="G3" s="23">
+        <v>12</v>
+      </c>
+      <c r="H3" s="23">
+        <v>70</v>
+      </c>
+      <c r="I3" s="30">
+        <v>41575</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3829,6 +3866,74 @@
       </c>
       <c r="F9" s="24">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="24.9" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="31" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3841,8 +3946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -3889,6 +3994,15 @@
       <c r="C2" t="s">
         <v>183</v>
       </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3899,6 +4013,15 @@
       </c>
       <c r="C3" t="s">
         <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3933,8 +4056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C22"/>
+    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>

</xml_diff>